<commit_message>
Add project Name variable extraction
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{15FF3B0C-523F-4127-93DE-22CE87CF292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{070099BA-5FC5-4646-869A-CEFDBC4F3149}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{15FF3B0C-523F-4127-93DE-22CE87CF292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1B6E71A-FC34-41EA-84C3-A4F453A790EB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Shub" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bpa!$A$1:$D$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bpa!$A$1:$D$141</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="190">
   <si>
     <t>Description</t>
   </si>
@@ -78,6 +78,9 @@
     <t>As built documents</t>
   </si>
   <si>
+    <t>As-Built Documentation soft and hard copies BF</t>
+  </si>
+  <si>
     <t>BF Fiber Deployment OSP- Duct Inspection Test on existing duct system (Mandrel, brush, pressure etc.)</t>
   </si>
   <si>
@@ -126,7 +129,7 @@
     <t>Units ISP Fiber Deployment- Installation of 1, 2, 4 core drop cable for ISP (Bend-Insensitive Fiber)Indoor/Outdoor drop cable Aramid Yam LSZH, G657A2</t>
   </si>
   <si>
-    <t xml:space="preserve">Installation of 1, 2, 4 core drop cable for ISP </t>
+    <t>Installation of 1, 2, 4 core drop cable for ISP</t>
   </si>
   <si>
     <t>BF Fiber Deployment OSP- Blowing upto 12-96 core Cable in existing Duct</t>
@@ -306,7 +309,7 @@
     <t>Units ISP Fiber Deployment- Supply &amp; Installation of cable tray width 50mm</t>
   </si>
   <si>
-    <t>Supply, Install and fix cable tray  50mm</t>
+    <t>Supply, Install and fix cable tray 50mm</t>
   </si>
   <si>
     <t>Units ISP Fiber Deployment- Supply &amp; Installation of cable tray width 100mm</t>
@@ -432,6 +435,9 @@
     <t>BATCH</t>
   </si>
   <si>
+    <t>Splicing, Testing and Commissioning 6-12 cores</t>
+  </si>
+  <si>
     <t>Aerial Fibre Deployment OSP- Installation of approved wooden pole (includes digging, pole erection &amp; ramming) (8m, 10m &amp; 12m)</t>
   </si>
   <si>
@@ -525,6 +531,9 @@
     <t>BF Fiber Deployment OSP- Construct and install Masonry Manhole, Cover and accessories (500x500x600mm)</t>
   </si>
   <si>
+    <t>Construct and install Masonry Manhole</t>
+  </si>
+  <si>
     <t>Units ISP Fiber Deployment- Installation of OLT</t>
   </si>
   <si>
@@ -604,9 +613,6 @@
   </si>
   <si>
     <t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</t>
-  </si>
-  <si>
-    <t>Construct and install Masonry Manhole</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864005FC-FDC6-4E63-9CE0-D0AB8CFD1612}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1109,35 +1115,35 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>5.28</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1146,40 +1152,40 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>23.23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1188,7 +1194,7 @@
         <v>23.23</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1199,7 +1205,10 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>23.23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1207,10 +1216,10 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>26.4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1232,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>30.8</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1243,21 +1252,21 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>36.96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1279,35 +1288,35 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>31</v>
+        <v>36.96</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
         <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1318,29 +1327,26 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>54.4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1349,7 +1355,7 @@
         <v>54.4</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1360,15 +1366,15 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>59.63</v>
+        <v>54.4</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1377,7 +1383,7 @@
         <v>59.63</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1385,21 +1391,24 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>64.010000000000005</v>
+        <v>59.63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
       <c r="C27">
-        <v>75</v>
+        <v>64.010000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1410,49 +1419,49 @@
         <v>8</v>
       </c>
       <c r="C28">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
         <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>85</v>
-      </c>
-      <c r="D29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>85</v>
+      </c>
+      <c r="D30" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
         <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1482,24 +1491,24 @@
         <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>150</v>
-      </c>
-      <c r="D34" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>150</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1521,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="C37">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1529,10 +1538,10 @@
         <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1543,21 +1552,21 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>264</v>
-      </c>
-      <c r="D39" t="s">
-        <v>62</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>264</v>
+      </c>
+      <c r="D40" t="s">
         <v>63</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1565,10 +1574,10 @@
         <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>366.08</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1576,10 +1585,10 @@
         <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C42">
-        <v>385.65</v>
+        <v>366.08</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1590,21 +1599,21 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>440</v>
-      </c>
-      <c r="D43" t="s">
-        <v>67</v>
+        <v>385.65</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44">
         <v>440</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1634,10 +1643,10 @@
         <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>488.4</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1645,38 +1654,38 @@
         <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>528</v>
-      </c>
-      <c r="D48" t="s">
-        <v>73</v>
+        <v>488.4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>528</v>
+      </c>
+      <c r="D49" t="s">
         <v>74</v>
-      </c>
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49">
-        <v>556.82000000000005</v>
-      </c>
-      <c r="D49" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>556.82000000000005</v>
+      </c>
+      <c r="D50" t="s">
         <v>76</v>
-      </c>
-      <c r="B50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50">
-        <v>600</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1687,21 +1696,21 @@
         <v>8</v>
       </c>
       <c r="C51">
-        <v>610.72</v>
-      </c>
-      <c r="D51" t="s">
-        <v>78</v>
+        <v>600</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>610.72</v>
+      </c>
+      <c r="D52" t="s">
         <v>79</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52">
-        <v>660</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1712,7 +1721,7 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>800</v>
+        <v>660</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1723,15 +1732,12 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>880</v>
-      </c>
-      <c r="D54" t="s">
-        <v>82</v>
+        <v>800</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -1740,18 +1746,21 @@
         <v>880</v>
       </c>
       <c r="D55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56">
         <v>880</v>
+      </c>
+      <c r="D56" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1759,24 +1768,24 @@
         <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>910</v>
-      </c>
-      <c r="D57" t="s">
-        <v>87</v>
+        <v>880</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>910</v>
+      </c>
+      <c r="D58" t="s">
         <v>88</v>
-      </c>
-      <c r="B58" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="7">
-        <v>1200</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1784,7 +1793,7 @@
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C59" s="7">
         <v>1200</v>
@@ -1798,7 +1807,7 @@
         <v>5</v>
       </c>
       <c r="C60" s="7">
-        <v>1250</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1822,19 +1831,19 @@
       <c r="C62" s="7">
         <v>1250</v>
       </c>
-      <c r="D62" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="7">
+        <v>1250</v>
+      </c>
+      <c r="D63" t="s">
         <v>94</v>
-      </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="7">
-        <v>1320</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1845,21 +1854,21 @@
         <v>5</v>
       </c>
       <c r="C64" s="7">
-        <v>1500</v>
-      </c>
-      <c r="D64" t="s">
-        <v>96</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="7">
         <v>1500</v>
+      </c>
+      <c r="D65" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -1870,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="7">
-        <v>1628</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -1878,38 +1887,38 @@
         <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C67" s="7">
-        <v>1800</v>
-      </c>
-      <c r="D67" t="s">
-        <v>100</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C68" s="7">
         <v>1800</v>
       </c>
       <c r="D68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="7">
+        <v>1800</v>
+      </c>
+      <c r="D69" t="s">
         <v>103</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="7">
-        <v>2000</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -1942,7 +1951,7 @@
         <v>5</v>
       </c>
       <c r="C72" s="7">
-        <v>2050</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -1950,10 +1959,10 @@
         <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C73" s="7">
-        <v>2100</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -1961,24 +1970,24 @@
         <v>108</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C74" s="7">
-        <v>2200</v>
-      </c>
-      <c r="D74" t="s">
-        <v>109</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="7">
         <v>2200</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
@@ -1991,33 +2000,33 @@
       <c r="C76" s="7">
         <v>2200</v>
       </c>
-      <c r="D76" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2200</v>
+      </c>
+      <c r="D77" t="s">
         <v>113</v>
-      </c>
-      <c r="B77" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="7">
-        <v>2300</v>
-      </c>
-      <c r="D77" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="7">
+        <v>2300</v>
+      </c>
+      <c r="D78" t="s">
         <v>115</v>
-      </c>
-      <c r="B78" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="7">
-        <v>2500</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -2025,7 +2034,7 @@
         <v>116</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C79" s="7">
         <v>2500</v>
@@ -2036,7 +2045,7 @@
         <v>117</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C80" s="7">
         <v>2500</v>
@@ -2050,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="C81" s="7">
-        <v>2640</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -2094,21 +2103,21 @@
         <v>5</v>
       </c>
       <c r="C85" s="7">
-        <v>2660</v>
-      </c>
-      <c r="D85" t="s">
-        <v>123</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>123</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="7">
+        <v>2660</v>
+      </c>
+      <c r="D86" t="s">
         <v>124</v>
-      </c>
-      <c r="B86" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="7">
-        <v>3000</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
@@ -2116,7 +2125,7 @@
         <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C87" s="7">
         <v>3000</v>
@@ -2138,26 +2147,29 @@
         <v>127</v>
       </c>
       <c r="B89" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C89" s="7">
-        <v>3300</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" t="s">
         <v>129</v>
       </c>
-      <c r="B90" t="s">
-        <v>5</v>
-      </c>
       <c r="C90" s="7">
-        <v>3500</v>
+        <v>3300</v>
+      </c>
+      <c r="D90" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
@@ -2168,27 +2180,24 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="7">
-        <v>3520</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="7">
-        <v>3960</v>
-      </c>
-      <c r="D93" t="s">
-        <v>133</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
@@ -2199,12 +2208,15 @@
         <v>5</v>
       </c>
       <c r="C94" s="7">
-        <v>4000</v>
+        <v>3960</v>
+      </c>
+      <c r="D94" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
@@ -2215,7 +2227,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B96" t="s">
         <v>5</v>
@@ -2226,7 +2238,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
@@ -2237,16 +2249,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="7">
-        <v>4400</v>
-      </c>
-      <c r="D98" t="s">
-        <v>139</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -2257,12 +2266,15 @@
         <v>5</v>
       </c>
       <c r="C99" s="7">
-        <v>4500</v>
+        <v>4400</v>
+      </c>
+      <c r="D99" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
@@ -2273,18 +2285,18 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="7">
-        <v>5000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B102" t="s">
         <v>5</v>
@@ -2295,7 +2307,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
@@ -2306,16 +2318,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C104" s="7">
-        <v>5280</v>
-      </c>
-      <c r="D104" t="s">
-        <v>146</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -2323,18 +2332,21 @@
         <v>147</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="C105" s="7">
-        <v>7500</v>
+        <v>5280</v>
+      </c>
+      <c r="D105" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C106" s="7">
         <v>7500</v>
@@ -2342,18 +2354,18 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="7">
-        <v>8000</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
@@ -2364,38 +2376,35 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B109" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="7">
-        <v>8500</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="7">
-        <v>8800</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B111" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="7">
-        <v>9000</v>
-      </c>
-      <c r="D111" t="s">
-        <v>154</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
@@ -2403,37 +2412,40 @@
         <v>155</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C112" s="7">
-        <v>9240</v>
+        <v>9000</v>
+      </c>
+      <c r="D112" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C113" s="7">
-        <v>9500</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="7">
-        <v>10500</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -2444,21 +2456,18 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
       </c>
       <c r="C116" s="7">
-        <v>11000</v>
-      </c>
-      <c r="D116" t="s">
-        <v>187</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
@@ -2466,10 +2475,13 @@
       <c r="C117" s="7">
         <v>11000</v>
       </c>
+      <c r="D117" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -2477,24 +2489,24 @@
       <c r="C118" s="7">
         <v>11000</v>
       </c>
-      <c r="D118" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
       </c>
       <c r="C119" s="7">
-        <v>13200</v>
+        <v>11000</v>
+      </c>
+      <c r="D119" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -2505,21 +2517,18 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
       </c>
       <c r="C121" s="7">
-        <v>13500</v>
-      </c>
-      <c r="D121" t="s">
-        <v>166</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -2528,7 +2537,7 @@
         <v>13500</v>
       </c>
       <c r="D122" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
@@ -2536,70 +2545,73 @@
         <v>168</v>
       </c>
       <c r="B123" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C123" s="7">
-        <v>14000</v>
+        <v>13500</v>
+      </c>
+      <c r="D123" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C124" s="7">
-        <v>15500</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B125" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C125" s="7">
-        <v>15840</v>
+        <v>15500</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C126" s="7">
-        <v>19500</v>
+        <v>15840</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
       </c>
       <c r="C127" s="7">
-        <v>19580</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
       </c>
       <c r="C128" s="7">
-        <v>20000</v>
+        <v>19580</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -2610,7 +2622,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -2621,7 +2633,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -2632,118 +2644,129 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B132" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C132" s="7">
-        <v>23760</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C133" s="7">
-        <v>24500</v>
+        <v>23760</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
       </c>
       <c r="C134" s="7">
-        <v>30800</v>
-      </c>
-      <c r="D134" t="s">
-        <v>180</v>
+        <v>24500</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
       </c>
       <c r="C135" s="7">
-        <v>36500</v>
+        <v>30800</v>
+      </c>
+      <c r="D135" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B136" t="s">
         <v>5</v>
       </c>
       <c r="C136" s="7">
-        <v>45760</v>
+        <v>36500</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C137" s="7">
-        <v>47520</v>
+        <v>45760</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C138" s="7">
-        <v>88000</v>
+        <v>47520</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="C139" s="7">
-        <v>95040</v>
+        <v>88000</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="C140" s="7">
+        <v>95040</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>189</v>
+      </c>
+      <c r="B141" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" s="7">
         <v>132000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D140" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D141" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7D0387-9D33-42A7-95B3-3BA9813FB715}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2802,6 +2825,13 @@
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
     </row>
+    <row r="11" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
     <row r="14" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
@@ -2809,12 +2839,26 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
+    <row r="16" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
     <row r="19" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2827,10 +2871,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.6328125" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2854,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5B91-39BE-4885-A0A9-44D289EC2A66}">
   <dimension ref="E2:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Extract Project name and Short Partner Name
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA1E3FC7-4134-4C99-97FC-B915207E06F8}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0525F0E7-6855-4337-A833-4FC10DD9068F}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="5" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="0" activeTab="0" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="BPADetails" sheetId="6" r:id="rId1"/>
     <x:sheet name="Bpa" sheetId="2" r:id="rId2"/>
     <x:sheet name="CmQuote" sheetId="1" r:id="rId3"/>
-    <x:sheet name="Linear" sheetId="4" r:id="rId4"/>
-    <x:sheet name="BrownField" sheetId="5" r:id="rId5"/>
-    <x:sheet name="Shub" sheetId="3" r:id="rId6"/>
+    <x:sheet name="Shub" sheetId="3" r:id="rId4"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BPADetails!$A$2:$A$17</x:definedName>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <x:si>
     <x:t>Partner</x:t>
   </x:si>
@@ -933,9 +931,6 @@
   </x:si>
   <x:si>
     <x:t>30,800.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UOM_1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1453,11 +1448,11 @@
   </x:sheetPr>
   <x:dimension ref="A1:E17"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C28" sqref="C28"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="101.874375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultColWidth="255" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
     <x:col min="1" max="1" width="11.90625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="8.816406" style="11" customWidth="1"/>
@@ -1772,9 +1767,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:D141"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="D1" sqref="D1 D:D"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
@@ -3491,14 +3484,18 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E20"/>
+  <x:dimension ref="A1:E23"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="E23" sqref="E23"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="47.816406" style="1" customWidth="1"/>
-    <x:col min="2" max="16384" width="8.726562" style="1" customWidth="1"/>
+    <x:col min="2" max="4" width="8.726562" style="1" customWidth="1"/>
+    <x:col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="16384" width="8.726562" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3654,7 +3651,7 @@
         <x:v>275</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A10" s="1" t="s">
         <x:v>196</x:v>
       </x:c>
@@ -3688,7 +3685,7 @@
         <x:v>278</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="12" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A12" s="1" t="s">
         <x:v>158</x:v>
       </x:c>
@@ -3705,7 +3702,7 @@
         <x:v>280</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A13" s="1" t="s">
         <x:v>174</x:v>
       </x:c>
@@ -3739,7 +3736,7 @@
         <x:v>284</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A15" s="1" t="s">
         <x:v>226</x:v>
       </x:c>
@@ -3790,7 +3787,7 @@
         <x:v>292</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="18" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A18" s="1" t="s">
         <x:v>144</x:v>
       </x:c>
@@ -3841,6 +3838,7 @@
         <x:v>295</x:v>
       </x:c>
     </x:row>
+    <x:row r="23" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3851,68 +3849,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{901F1140-F679-43DE-9DAA-589194A5394A}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A18" sqref="A18"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <x:cols>
-    <x:col min="1" max="1" width="44.632812" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData/>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{CBEF88CE-4F1B-471B-B445-815061B09B12}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView topLeftCell="A2" workbookViewId="0">
-      <x:selection activeCell="G22" sqref="G22 G21:G22"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <x:sheetData/>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{C0BA5B91-39BE-4885-A0A9-44D289EC2A66}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="C2:F2"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G7" sqref="G7"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
-    <x:col min="1" max="1" width="28.90625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="36.269531" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="9.179688" style="0" customWidth="1"/>
-    <x:col min="3" max="4" width="9.179688" style="17" customWidth="1"/>
-    <x:col min="5" max="5" width="10.726562" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="17.179688" style="17" customWidth="1"/>
+    <x:col min="3" max="3" width="11.542969" style="17" customWidth="1"/>
+    <x:col min="4" max="4" width="10.542969" style="17" customWidth="1"/>
+    <x:col min="5" max="5" width="12" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="52" style="17" customWidth="1"/>
     <x:col min="7" max="8" width="9.179688" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="5.816406" style="0" bestFit="1" customWidth="1"/>
     <x:col min="10" max="10" width="9.179688" style="0" customWidth="1"/>
@@ -3920,585 +3874,8 @@
     <x:col min="12" max="13" width="11.632812" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:13">
-      <x:c r="A1" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C1" s="17" t="s">
-        <x:v>252</x:v>
-      </x:c>
-      <x:c r="D1" s="17" t="s">
-        <x:v>253</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>254</x:v>
-      </x:c>
-      <x:c r="F1" s="17" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-    </x:row>
     <x:row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C2" s="17" t="s">
-        <x:v>269</x:v>
-      </x:c>
-      <x:c r="D2" s="17" t="s">
-        <x:v>270</x:v>
-      </x:c>
-      <x:c r="E2" s="7" t="s">
-        <x:v>271</x:v>
-      </x:c>
-      <x:c r="F2" s="17" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="n">
-        <x:v>5.28</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:13">
-      <x:c r="A3" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C3" s="17" t="s">
-        <x:v>272</x:v>
-      </x:c>
-      <x:c r="D3" s="17" t="s">
-        <x:v>270</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>273</x:v>
-      </x:c>
-      <x:c r="F3" s="17" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="n">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:13">
-      <x:c r="A4" s="0" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C4" s="17" t="s">
-        <x:v>256</x:v>
-      </x:c>
-      <x:c r="D4" s="17" t="s">
-        <x:v>257</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>258</x:v>
-      </x:c>
-      <x:c r="F4" s="17" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="n">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="s">
-        <x:v>93</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:13">
-      <x:c r="A5" s="0" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C5" s="17" t="s">
-        <x:v>274</x:v>
-      </x:c>
-      <x:c r="D5" s="17" t="s">
-        <x:v>270</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>275</x:v>
-      </x:c>
-      <x:c r="F5" s="17" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="n">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
-        <x:v>98</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:13">
-      <x:c r="A6" s="0" t="s">
-        <x:v>109</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C6" s="17" t="s">
-        <x:v>263</x:v>
-      </x:c>
-      <x:c r="D6" s="17" t="s">
-        <x:v>264</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>265</x:v>
-      </x:c>
-      <x:c r="F6" s="17" t="s">
-        <x:v>108</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="n">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>109</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:13">
-      <x:c r="A7" s="0" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>255</x:v>
-      </x:c>
-      <x:c r="C7" s="17" t="s">
-        <x:v>266</x:v>
-      </x:c>
-      <x:c r="D7" s="17" t="s">
-        <x:v>267</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>268</x:v>
-      </x:c>
-      <x:c r="F7" s="17" t="s">
-        <x:v>112</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="n">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="s">
-        <x:v>113</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:13">
-      <x:c r="A8" s="0" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C8" s="17" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="D8" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="F8" s="17" t="s">
-        <x:v>134</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="n">
-        <x:v>528</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
-        <x:v>135</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:13">
-      <x:c r="A9" s="0" t="s">
-        <x:v>144</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C9" s="17" t="s">
-        <x:v>293</x:v>
-      </x:c>
-      <x:c r="D9" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>293</x:v>
-      </x:c>
-      <x:c r="F9" s="17" t="s">
-        <x:v>143</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="n">
-        <x:v>880</x:v>
-      </x:c>
-      <x:c r="I9" s="0" t="s">
-        <x:v>144</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:13">
-      <x:c r="A10" s="0" t="s">
-        <x:v>155</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C10" s="17" t="s">
-        <x:v>287</x:v>
-      </x:c>
-      <x:c r="D10" s="17" t="s">
-        <x:v>288</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>289</x:v>
-      </x:c>
-      <x:c r="F10" s="17" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="G10" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H10" s="0" t="n">
-        <x:v>1250</x:v>
-      </x:c>
-      <x:c r="I10" s="0" t="s">
-        <x:v>155</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:13">
-      <x:c r="A11" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C11" s="17" t="s">
-        <x:v>279</x:v>
-      </x:c>
-      <x:c r="D11" s="17" t="s">
-        <x:v>267</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>280</x:v>
-      </x:c>
-      <x:c r="F11" s="17" t="s">
-        <x:v>157</x:v>
-      </x:c>
-      <x:c r="G11" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H11" s="0" t="n">
-        <x:v>1500</x:v>
-      </x:c>
-      <x:c r="I11" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:13">
-      <x:c r="A12" s="0" t="s">
-        <x:v>164</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C12" s="17" t="s">
-        <x:v>282</x:v>
-      </x:c>
-      <x:c r="D12" s="17" t="s">
-        <x:v>283</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>284</x:v>
-      </x:c>
-      <x:c r="F12" s="17" t="s">
-        <x:v>163</x:v>
-      </x:c>
-      <x:c r="G12" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H12" s="0" t="n">
-        <x:v>1800</x:v>
-      </x:c>
-      <x:c r="I12" s="0" t="s">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:13">
-      <x:c r="A13" s="0" t="s">
-        <x:v>171</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C13" s="17" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="D13" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="F13" s="17" t="s">
-        <x:v>170</x:v>
-      </x:c>
-      <x:c r="G13" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H13" s="0" t="n">
-        <x:v>2200</x:v>
-      </x:c>
-      <x:c r="I13" s="0" t="s">
-        <x:v>171</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:13">
-      <x:c r="A14" s="0" t="s">
-        <x:v>174</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C14" s="17" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="D14" s="17" t="s">
-        <x:v>267</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>281</x:v>
-      </x:c>
-      <x:c r="F14" s="17" t="s">
-        <x:v>173</x:v>
-      </x:c>
-      <x:c r="G14" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H14" s="0" t="n">
-        <x:v>2200</x:v>
-      </x:c>
-      <x:c r="I14" s="0" t="s">
-        <x:v>174</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:13">
-      <x:c r="A15" s="0" t="s">
-        <x:v>176</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C15" s="17" t="s">
-        <x:v>290</x:v>
-      </x:c>
-      <x:c r="D15" s="17" t="s">
-        <x:v>291</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>292</x:v>
-      </x:c>
-      <x:c r="F15" s="17" t="s">
-        <x:v>175</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H15" s="0" t="n">
-        <x:v>2300</x:v>
-      </x:c>
-      <x:c r="I15" s="0" t="s">
-        <x:v>176</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:13">
-      <x:c r="A16" s="0" t="s">
-        <x:v>196</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C16" s="17" t="s">
-        <x:v>276</x:v>
-      </x:c>
-      <x:c r="D16" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>276</x:v>
-      </x:c>
-      <x:c r="F16" s="17" t="s">
-        <x:v>195</x:v>
-      </x:c>
-      <x:c r="G16" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H16" s="0" t="n">
-        <x:v>3960</x:v>
-      </x:c>
-      <x:c r="I16" s="0" t="s">
-        <x:v>196</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:13">
-      <x:c r="A17" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C17" s="17" t="s">
-        <x:v>294</x:v>
-      </x:c>
-      <x:c r="D17" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
-      <x:c r="F17" s="17" t="s">
-        <x:v>201</x:v>
-      </x:c>
-      <x:c r="G17" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H17" s="0" t="n">
-        <x:v>4400</x:v>
-      </x:c>
-      <x:c r="I17" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:13">
-      <x:c r="A18" s="0" t="s">
-        <x:v>226</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C18" s="17" t="s">
-        <x:v>285</x:v>
-      </x:c>
-      <x:c r="D18" s="17" t="s">
-        <x:v>283</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>286</x:v>
-      </x:c>
-      <x:c r="F18" s="17" t="s">
-        <x:v>225</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H18" s="0" t="n">
-        <x:v>11000</x:v>
-      </x:c>
-      <x:c r="I18" s="0" t="s">
-        <x:v>226</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:13">
-      <x:c r="A19" s="0" t="s">
-        <x:v>230</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C19" s="17" t="s">
-        <x:v>277</x:v>
-      </x:c>
-      <x:c r="D19" s="17" t="s">
-        <x:v>264</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>278</x:v>
-      </x:c>
-      <x:c r="F19" s="17" t="s">
-        <x:v>229</x:v>
-      </x:c>
-      <x:c r="G19" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H19" s="0" t="n">
-        <x:v>13500</x:v>
-      </x:c>
-      <x:c r="I19" s="0" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:13">
-      <x:c r="A20" s="0" t="s">
-        <x:v>244</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>259</x:v>
-      </x:c>
-      <x:c r="C20" s="17" t="s">
-        <x:v>295</x:v>
-      </x:c>
-      <x:c r="D20" s="17" t="s">
-        <x:v>261</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>295</x:v>
-      </x:c>
-      <x:c r="F20" s="17" t="s">
-        <x:v>243</x:v>
-      </x:c>
-      <x:c r="G20" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="H20" s="0" t="n">
-        <x:v>30800</x:v>
-      </x:c>
-      <x:c r="I20" s="0" t="s">
-        <x:v>244</x:v>
-      </x:c>
+      <x:c r="E2" s="7" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Updated BPA translator to point to correct variables
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
   <x:si>
     <x:t>Partner</x:t>
   </x:si>
@@ -808,6 +808,9 @@
   </x:si>
   <x:si>
     <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oracle Description</x:t>
   </x:si>
   <x:si>
     <x:t>m</x:t>
@@ -3498,7 +3501,7 @@
     <x:col min="6" max="16384" width="8.726562" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A1" s="15" t="s">
         <x:v>251</x:v>
       </x:c>
@@ -3514,331 +3517,391 @@
       <x:c r="E1" s="1" t="s">
         <x:v>254</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="F1" s="1" t="s">
+        <x:v>255</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="2" t="s">
         <x:v>93</x:v>
       </x:c>
       <x:c r="B2" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="D2" s="5" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="E2" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
+        <x:v>92</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A3" s="2" t="s">
         <x:v>135</x:v>
       </x:c>
       <x:c r="B3" s="3" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C3" s="4" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="D3" s="5" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
         <x:v>261</x:v>
       </x:c>
-      <x:c r="E3" s="1" t="s">
-        <x:v>260</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="F3" s="1" t="s">
+        <x:v>134</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A4" s="2" t="s">
         <x:v>171</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="D4" s="5" t="s">
         <x:v>262</x:v>
       </x:c>
-      <x:c r="D4" s="5" t="s">
-        <x:v>261</x:v>
-      </x:c>
       <x:c r="E4" s="1" t="s">
-        <x:v>262</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="F4" s="1" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A5" s="2" t="s">
         <x:v>109</x:v>
       </x:c>
       <x:c r="B5" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="D5" s="5" t="s">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="E5" s="1" t="s">
-        <x:v>265</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="F5" s="1" t="s">
+        <x:v>108</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A6" s="2" t="s">
         <x:v>113</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="D6" s="5" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="E6" s="1" t="s">
-        <x:v>268</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="F6" s="1" t="s">
+        <x:v>112</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A7" s="2" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="D7" s="4" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E7" s="1" t="s">
-        <x:v>271</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F7" s="1" t="s">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A8" s="1" t="s">
         <x:v>76</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="D8" s="1" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E8" s="1" t="s">
-        <x:v>273</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="F8" s="1" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A9" s="1" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="D9" s="1" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E9" s="1" t="s">
-        <x:v>275</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="F9" s="1" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A10" s="1" t="s">
         <x:v>196</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="D10" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E10" s="1" t="s">
-        <x:v>276</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="F10" s="1" t="s">
+        <x:v>195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A11" s="1" t="s">
         <x:v>230</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="D11" s="1" t="s">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="E11" s="1" t="s">
-        <x:v>278</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="F11" s="1" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A12" s="1" t="s">
         <x:v>158</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="E12" s="1" t="s">
-        <x:v>280</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="F12" s="1" t="s">
+        <x:v>157</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A13" s="1" t="s">
         <x:v>174</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="E13" s="1" t="s">
-        <x:v>281</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="F13" s="1" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A14" s="1" t="s">
         <x:v>164</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="E14" s="1" t="s">
-        <x:v>284</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="F14" s="1" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A15" s="1" t="s">
         <x:v>226</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="E15" s="1" t="s">
-        <x:v>286</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F15" s="1" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A16" s="1" t="s">
         <x:v>155</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D16" s="1" t="s">
-        <x:v>288</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E16" s="1" t="s">
-        <x:v>289</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F16" s="1" t="s">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A17" s="1" t="s">
         <x:v>176</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="E17" s="1" t="s">
-        <x:v>292</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="F17" s="1" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A18" s="1" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="D18" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E18" s="1" t="s">
-        <x:v>293</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="F18" s="1" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A19" s="1" t="s">
         <x:v>202</x:v>
       </x:c>
       <x:c r="B19" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C19" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="D19" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E19" s="1" t="s">
-        <x:v>294</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="F19" s="1" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A20" s="1" t="s">
         <x:v>244</x:v>
       </x:c>
       <x:c r="B20" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C20" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="D20" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E20" s="1" t="s">
-        <x:v>295</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="F20" s="1" t="s">
+        <x:v>243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3874,8 +3937,405 @@
     <x:col min="12" max="13" width="11.632812" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
+    <x:row r="1" spans="1:13">
+      <x:c r="A1" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C1" s="17" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="D1" s="17" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="F1" s="17" t="s">
+        <x:v>255</x:v>
+      </x:c>
+    </x:row>
     <x:row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <x:c r="E2" s="7" t="s"/>
+      <x:c r="A2" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C2" s="17" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="D2" s="17" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="E2" s="7" t="s">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="F2" s="17" t="s">
+        <x:v>92</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:13">
+      <x:c r="A3" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C3" s="17" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="D3" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F3" s="17" t="s">
+        <x:v>134</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:13">
+      <x:c r="A4" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C4" s="17" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="D4" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="F4" s="17" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:13">
+      <x:c r="A5" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C5" s="17" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="D5" s="17" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="F5" s="17" t="s">
+        <x:v>108</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:13">
+      <x:c r="A6" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C6" s="17" t="s">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="D6" s="17" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="F6" s="17" t="s">
+        <x:v>112</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:13">
+      <x:c r="A7" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C7" s="17" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="D7" s="17" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F7" s="17" t="s">
+        <x:v>70</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:13">
+      <x:c r="A8" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C8" s="17" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="D8" s="17" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="F8" s="17" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:13">
+      <x:c r="A9" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C9" s="17" t="s">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="D9" s="17" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="F9" s="17" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:13">
+      <x:c r="A10" s="0" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C10" s="17" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="D10" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="F10" s="17" t="s">
+        <x:v>195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:13">
+      <x:c r="A11" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C11" s="17" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="D11" s="17" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="F11" s="17" t="s">
+        <x:v>229</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:13">
+      <x:c r="A12" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C12" s="17" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="D12" s="17" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="F12" s="17" t="s">
+        <x:v>157</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:13">
+      <x:c r="A13" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C13" s="17" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="D13" s="17" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="F13" s="17" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:13">
+      <x:c r="A14" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C14" s="17" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="D14" s="17" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="F14" s="17" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:13">
+      <x:c r="A15" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C15" s="17" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="D15" s="17" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F15" s="17" t="s">
+        <x:v>225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:13">
+      <x:c r="A16" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C16" s="17" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="D16" s="17" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F16" s="17" t="s">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:13">
+      <x:c r="A17" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C17" s="17" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="D17" s="17" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="F17" s="17" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:13">
+      <x:c r="A18" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C18" s="17" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="D18" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="F18" s="17" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:13">
+      <x:c r="A19" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C19" s="17" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="D19" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="F19" s="17" t="s">
+        <x:v>201</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:13">
+      <x:c r="A20" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C20" s="17" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="D20" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="F20" s="17" t="s">
+        <x:v>243</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Replaced PDF Data extraction workflow
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0525F0E7-6855-4337-A833-4FC10DD9068F}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3F63D70-F586-4378-A0D6-19D5A2B8D8B4}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="0" activeTab="0" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="3" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <x:si>
     <x:t>Partner</x:t>
   </x:si>
@@ -819,10 +819,10 @@
     <x:t>43.00</x:t>
   </x:si>
   <x:si>
-    <x:t>3704</x:t>
-  </x:si>
-  <x:si>
-    <x:t>159,272.00</x:t>
+    <x:t>510</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21,930.00</x:t>
   </x:si>
   <x:si>
     <x:t>pce</x:t>
@@ -834,106 +834,103 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
+    <x:t>5.28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>397</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,096.16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6,352.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18,659.00</x:t>
+  </x:si>
+  <x:si>
     <x:t>2,200.00</x:t>
   </x:si>
   <x:si>
-    <x:t>80.00</x:t>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,400.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,800.00</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>400.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>90.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>900.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3442</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18,173.76</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>55,072.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>47.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>161,774.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3,960.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13,500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>67,500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1,500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15,000.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22,000.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1,800.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>45,000.00</x:t>
-  </x:si>
-  <x:si>
     <x:t>11,000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>275,000.00</x:t>
+    <x:t>55,000.00</x:t>
   </x:si>
   <x:si>
     <x:t>1,250.00</x:t>
   </x:si>
   <x:si>
-    <x:t>43</x:t>
-  </x:si>
-  <x:si>
-    <x:t>53,750.00</x:t>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7,500.00</x:t>
   </x:si>
   <x:si>
     <x:t>2,300.00</x:t>
   </x:si>
   <x:si>
-    <x:t>86</x:t>
-  </x:si>
-  <x:si>
-    <x:t>197,800.00</x:t>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27,600.00</x:t>
   </x:si>
   <x:si>
     <x:t>880.00</x:t>
   </x:si>
   <x:si>
-    <x:t>4,400.00</x:t>
-  </x:si>
-  <x:si>
     <x:t>30,800.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Brown Field :</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 275,525.16</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1451,7 +1448,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:E17"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="C28" sqref="C28"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1770,7 +1767,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:D141"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView topLeftCell="A4" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
@@ -3487,13 +3484,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E23"/>
+  <x:dimension ref="A1:F23"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E23" sqref="E23"/>
+      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
     <x:col min="1" max="1" width="47.816406" style="1" customWidth="1"/>
     <x:col min="2" max="4" width="8.726562" style="1" customWidth="1"/>
@@ -3563,70 +3560,70 @@
     </x:row>
     <x:row r="4" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A4" s="2" t="s">
-        <x:v>171</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
-        <x:v>260</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
         <x:v>263</x:v>
       </x:c>
       <x:c r="D4" s="5" t="s">
-        <x:v>262</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E4" s="1" t="s">
-        <x:v>263</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F4" s="1" t="s">
-        <x:v>170</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A5" s="2" t="s">
-        <x:v>109</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B5" s="3" t="s">
         <x:v>256</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D5" s="5" t="s">
         <x:v>264</x:v>
       </x:c>
-      <x:c r="D5" s="5" t="s">
-        <x:v>265</x:v>
-      </x:c>
       <x:c r="E5" s="1" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F5" s="1" t="s">
-        <x:v>108</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A6" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
         <x:v>256</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="D6" s="5" t="s">
-        <x:v>268</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E6" s="1" t="s">
         <x:v>269</x:v>
       </x:c>
       <x:c r="F6" s="1" t="s">
-        <x:v>112</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A7" s="2" t="s">
-        <x:v>71</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
         <x:v>270</x:v>
@@ -3638,269 +3635,238 @@
         <x:v>272</x:v>
       </x:c>
       <x:c r="F7" s="1" t="s">
-        <x:v>70</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A8" s="1" t="s">
-        <x:v>76</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
         <x:v>273</x:v>
       </x:c>
       <x:c r="D8" s="1" t="s">
-        <x:v>271</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E8" s="1" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="F8" s="1" t="s">
-        <x:v>75</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A9" s="1" t="s">
-        <x:v>98</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="D9" s="1" t="s">
-        <x:v>271</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E9" s="1" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="F9" s="1" t="s">
-        <x:v>97</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A10" s="1" t="s">
-        <x:v>196</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="D10" s="1" t="s">
-        <x:v>262</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="E10" s="1" t="s">
-        <x:v>277</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="F10" s="1" t="s">
-        <x:v>195</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A11" s="1" t="s">
-        <x:v>230</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>278</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="D11" s="1" t="s">
-        <x:v>265</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E11" s="1" t="s">
-        <x:v>279</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F11" s="1" t="s">
-        <x:v>229</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A12" s="1" t="s">
-        <x:v>158</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>280</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
-        <x:v>268</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E12" s="1" t="s">
-        <x:v>281</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F12" s="1" t="s">
-        <x:v>157</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A13" s="1" t="s">
-        <x:v>174</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
-        <x:v>263</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>268</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E13" s="1" t="s">
-        <x:v>282</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="F13" s="1" t="s">
-        <x:v>173</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A14" s="1" t="s">
-        <x:v>164</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>284</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E14" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="F14" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A15" s="1" t="s">
-        <x:v>226</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>286</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>284</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E15" s="1" t="s">
-        <x:v>287</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F15" s="1" t="s">
-        <x:v>225</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A16" s="1" t="s">
-        <x:v>155</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>288</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="D16" s="1" t="s">
-        <x:v>289</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E16" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F16" s="1" t="s">
-        <x:v>154</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A17" s="1" t="s">
-        <x:v>176</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E17" s="1" t="s">
         <x:v>292</x:v>
       </x:c>
-      <x:c r="E17" s="1" t="s">
-        <x:v>293</x:v>
-      </x:c>
       <x:c r="F17" s="1" t="s">
-        <x:v>175</x:v>
+        <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A18" s="1" t="s">
-        <x:v>144</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="D18" s="1" t="s">
-        <x:v>262</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E18" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F18" s="1" t="s">
-        <x:v>143</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A19" s="1" t="s">
-        <x:v>202</x:v>
-      </x:c>
-      <x:c r="B19" s="1" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="C19" s="1" t="s">
-        <x:v>295</x:v>
-      </x:c>
-      <x:c r="D19" s="1" t="s">
-        <x:v>262</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="E19" s="1" t="s">
         <x:v>295</x:v>
       </x:c>
-      <x:c r="F19" s="1" t="s">
-        <x:v>201</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <x:c r="A20" s="1" t="s">
-        <x:v>244</x:v>
-      </x:c>
-      <x:c r="B20" s="1" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="C20" s="1" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="D20" s="1" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="E20" s="1" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="F20" s="1" t="s">
-        <x:v>243</x:v>
-      </x:c>
-    </x:row>
+    </x:row>
+    <x:row r="20" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <x:row r="23" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -3918,8 +3884,8 @@
   </x:sheetPr>
   <x:dimension ref="C2:F2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E12" sqref="E12"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3999,70 +3965,70 @@
     </x:row>
     <x:row r="4" spans="1:13">
       <x:c r="A4" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C4" s="17" t="s">
         <x:v>263</x:v>
       </x:c>
       <x:c r="D4" s="17" t="s">
-        <x:v>262</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="F4" s="17" t="s">
-        <x:v>170</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:13">
       <x:c r="A5" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>256</x:v>
       </x:c>
       <x:c r="C5" s="17" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D5" s="17" t="s">
         <x:v>264</x:v>
       </x:c>
-      <x:c r="D5" s="17" t="s">
-        <x:v>265</x:v>
-      </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="F5" s="17" t="s">
-        <x:v>108</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:13">
       <x:c r="A6" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>256</x:v>
       </x:c>
       <x:c r="C6" s="17" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="D6" s="17" t="s">
-        <x:v>268</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>269</x:v>
       </x:c>
       <x:c r="F6" s="17" t="s">
-        <x:v>112</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:13">
       <x:c r="A7" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C7" s="17" t="s">
         <x:v>270</x:v>
@@ -4074,268 +4040,239 @@
         <x:v>272</x:v>
       </x:c>
       <x:c r="F7" s="17" t="s">
-        <x:v>70</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:13">
       <x:c r="A8" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C8" s="17" t="s">
         <x:v>273</x:v>
       </x:c>
       <x:c r="D8" s="17" t="s">
-        <x:v>271</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="F8" s="17" t="s">
-        <x:v>75</x:v>
+        <x:v>157</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:13">
       <x:c r="A9" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C9" s="17" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="D9" s="17" t="s">
-        <x:v>271</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="F9" s="17" t="s">
-        <x:v>97</x:v>
+        <x:v>216</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:13">
       <x:c r="A10" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C10" s="17" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="D10" s="17" t="s">
-        <x:v>262</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="F10" s="17" t="s">
-        <x:v>195</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:13">
       <x:c r="A11" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="17" t="s">
-        <x:v>278</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="D11" s="17" t="s">
-        <x:v>265</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>279</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="F11" s="17" t="s">
-        <x:v>229</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:13">
       <x:c r="A12" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="17" t="s">
-        <x:v>280</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D12" s="17" t="s">
-        <x:v>268</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="F12" s="17" t="s">
-        <x:v>157</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:13">
       <x:c r="A13" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="17" t="s">
-        <x:v>263</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="D13" s="17" t="s">
-        <x:v>268</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="F13" s="17" t="s">
-        <x:v>173</x:v>
+        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:13">
       <x:c r="A14" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="17" t="s">
-        <x:v>283</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D14" s="17" t="s">
-        <x:v>284</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="F14" s="17" t="s">
-        <x:v>163</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:13">
       <x:c r="A15" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="17" t="s">
-        <x:v>286</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D15" s="17" t="s">
-        <x:v>284</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F15" s="17" t="s">
-        <x:v>225</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:13">
       <x:c r="A16" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="17" t="s">
-        <x:v>288</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="D16" s="17" t="s">
-        <x:v>289</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>290</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="F16" s="17" t="s">
-        <x:v>154</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:13">
       <x:c r="A17" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="17" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D17" s="17" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
         <x:v>292</x:v>
       </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>293</x:v>
-      </x:c>
       <x:c r="F17" s="17" t="s">
-        <x:v>175</x:v>
+        <x:v>243</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:13">
       <x:c r="A18" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C18" s="17" t="s">
-        <x:v>294</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="D18" s="17" t="s">
-        <x:v>262</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>294</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="F18" s="17" t="s">
-        <x:v>143</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:13">
       <x:c r="A19" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="C19" s="17" t="s">
-        <x:v>295</x:v>
-      </x:c>
-      <x:c r="D19" s="17" t="s">
-        <x:v>262</x:v>
-      </x:c>
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="C19" s="17" t="s"/>
+      <x:c r="D19" s="17" t="s"/>
       <x:c r="E19" s="0" t="s">
         <x:v>295</x:v>
       </x:c>
-      <x:c r="F19" s="17" t="s">
-        <x:v>201</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:13">
-      <x:c r="A20" s="0" t="s">
-        <x:v>244</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>260</x:v>
-      </x:c>
-      <x:c r="C20" s="17" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="D20" s="17" t="s">
-        <x:v>262</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="F20" s="17" t="s">
-        <x:v>243</x:v>
-      </x:c>
+      <x:c r="F19" s="17" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Point to Input Directory to store extracted CM_Quote
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3F63D70-F586-4378-A0D6-19D5A2B8D8B4}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF0A5A44-313E-4F73-852A-40991F1F4B40}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </bookViews>
   <sheets>
     <sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="251">
   <si>
     <t>Partner</t>
   </si>
@@ -796,141 +796,6 @@
   </si>
   <si>
     <t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</t>
-  </si>
-  <si>
-    <t>Item Description</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Oracle Description</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>43.00</t>
-  </si>
-  <si>
-    <t>510</t>
-  </si>
-  <si>
-    <t>21,930.00</t>
-  </si>
-  <si>
-    <t>pce</t>
-  </si>
-  <si>
-    <t>528.00</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5.28</t>
-  </si>
-  <si>
-    <t>397</t>
-  </si>
-  <si>
-    <t>2,096.16</t>
-  </si>
-  <si>
-    <t>16.00</t>
-  </si>
-  <si>
-    <t>6,352.00</t>
-  </si>
-  <si>
-    <t>47.00</t>
-  </si>
-  <si>
-    <t>18,659.00</t>
-  </si>
-  <si>
-    <t>2,200.00</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4,400.00</t>
-  </si>
-  <si>
-    <t>1,500.00</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4,500.00</t>
-  </si>
-  <si>
-    <t>9,000.00</t>
-  </si>
-  <si>
-    <t>27,000.00</t>
-  </si>
-  <si>
-    <t>13,500.00</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>54,000.00</t>
-  </si>
-  <si>
-    <t>1,800.00</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>11,000.00</t>
-  </si>
-  <si>
-    <t>55,000.00</t>
-  </si>
-  <si>
-    <t>1,250.00</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7,500.00</t>
-  </si>
-  <si>
-    <t>2,300.00</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>27,600.00</t>
-  </si>
-  <si>
-    <t>880.00</t>
-  </si>
-  <si>
-    <t>30,800.00</t>
-  </si>
-  <si>
-    <t>440.00</t>
-  </si>
-  <si>
-    <t>Total Brown Field :</t>
-  </si>
-  <si>
-    <t>Ksh 275,525.16</t>
   </si>
 </sst>
 </file>
@@ -983,7 +848,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -993,12 +858,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1042,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1077,7 +936,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1394,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FBFE2F-7015-4DE4-93BF-E8592BA26E47}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -3419,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7D0387-9D33-42A7-95B3-3BA9813FB715}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1 A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3433,372 +3294,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>255</v>
-      </c>
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>229</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>163</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>225</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>295</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3810,10 +3451,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5B91-39BE-4885-A0A9-44D289EC2A66}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="C2:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3822,7 +3463,7 @@
     <col min="2" max="2" width="9.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="14" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12" style="16" customWidth="1"/>
     <col min="6" max="6" width="52" style="14" customWidth="1"/>
     <col min="7" max="8" width="9.1796875" customWidth="1"/>
     <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
@@ -3831,373 +3472,8 @@
     <col min="12" max="13" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="E3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="E4" t="s">
-        <v>265</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="E6" t="s">
-        <v>269</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="E7" t="s">
-        <v>272</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="E8" t="s">
-        <v>275</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" t="s">
-        <v>277</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="E10" t="s">
-        <v>280</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" t="s">
-        <v>260</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="E11" t="s">
-        <v>276</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" t="s">
-        <v>260</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="E12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" t="s">
-        <v>260</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" t="s">
-        <v>287</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" t="s">
-        <v>260</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" t="s">
-        <v>290</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" t="s">
-        <v>260</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="E15" t="s">
-        <v>291</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="E16" t="s">
-        <v>272</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>244</v>
-      </c>
-      <c r="B17" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="E17" t="s">
-        <v>292</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>260</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="E18" t="s">
-        <v>291</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>294</v>
-      </c>
-      <c r="E19" t="s">
-        <v>295</v>
-      </c>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Convert Short Partner Name to Upper case for proper corelation with BPA details table.
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{801AFBC9-5A1D-44F3-BA0E-8E5DB8F2EDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF0A5A44-313E-4F73-852A-40991F1F4B40}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{313948B6-BDCC-4361-8F1F-2DCF3F1DC5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C85E1D-73FA-489A-AE79-EE60CC216505}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </bookViews>
   <sheets>
     <sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Agreement 516313</t>
   </si>
   <si>
-    <t>Kinde</t>
-  </si>
-  <si>
     <t>KINDE ENGINEERING WORKS LIMITED</t>
   </si>
   <si>
@@ -96,16 +93,13 @@
     <t>Agreement 516306</t>
   </si>
   <si>
-    <t>Camusat</t>
-  </si>
-  <si>
     <t>CAMUSAT KENYA LIMITED</t>
   </si>
   <si>
     <t>Agreement 514807</t>
   </si>
   <si>
-    <t>Egypro</t>
+    <t>EGYPRO</t>
   </si>
   <si>
     <t>EGYPRO EAST AFRICA LTD</t>
@@ -117,36 +111,24 @@
     <t>Agreement 516301</t>
   </si>
   <si>
-    <t>Extra D</t>
-  </si>
-  <si>
     <t>EXTRA DIMENSIONS COMPANY LIMITED</t>
   </si>
   <si>
     <t>Agreement 522921</t>
   </si>
   <si>
-    <t>Tetranet</t>
-  </si>
-  <si>
     <t>TETRANET SERVICES LIMITED</t>
   </si>
   <si>
     <t>Agreement 516311</t>
   </si>
   <si>
-    <t>Adrian</t>
-  </si>
-  <si>
     <t>ADRIAN KENYA LIMITED</t>
   </si>
   <si>
     <t>Agreement 516300</t>
   </si>
   <si>
-    <t>Pavicon</t>
-  </si>
-  <si>
     <t>PAVICON (K) LIMITED</t>
   </si>
   <si>
@@ -156,9 +138,6 @@
     <t>Agreement 516303</t>
   </si>
   <si>
-    <t>Hatikvah</t>
-  </si>
-  <si>
     <t>HATIKVAH COMMUNICATIONS &amp; GENERAL ENGINEERING LIMITED</t>
   </si>
   <si>
@@ -168,9 +147,6 @@
     <t>Agreement 516305</t>
   </si>
   <si>
-    <t>Optimax</t>
-  </si>
-  <si>
     <t>OPTIMAX GROUP LIMITED</t>
   </si>
   <si>
@@ -180,9 +156,6 @@
     <t>Agreement 516302</t>
   </si>
   <si>
-    <t>Techminds</t>
-  </si>
-  <si>
     <t>TECHMINDS TECHNOLOGIES</t>
   </si>
   <si>
@@ -192,16 +165,13 @@
     <t>Agreement 516315</t>
   </si>
   <si>
-    <t>Powergen</t>
-  </si>
-  <si>
     <t>POWERGEN TECHNOLOGIES LTD</t>
   </si>
   <si>
     <t>Agreement 516312</t>
   </si>
   <si>
-    <t>Fireside</t>
+    <t>FIRESIDE</t>
   </si>
   <si>
     <t>FIRESIDE COMMUNICATIONS LIMITED</t>
@@ -210,9 +180,6 @@
     <t>Agreement 516304</t>
   </si>
   <si>
-    <t>Huawei</t>
-  </si>
-  <si>
     <t>HUAWEI TECHNOLOGIES(KENYA) CO. LTD</t>
   </si>
   <si>
@@ -796,6 +763,39 @@
   </si>
   <si>
     <t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</t>
+  </si>
+  <si>
+    <t>KINDE</t>
+  </si>
+  <si>
+    <t>CAMUSAT</t>
+  </si>
+  <si>
+    <t>EXTRA D</t>
+  </si>
+  <si>
+    <t>TETRANET</t>
+  </si>
+  <si>
+    <t>ADRIAN</t>
+  </si>
+  <si>
+    <t>PAVICON</t>
+  </si>
+  <si>
+    <t>HATIKVAH</t>
+  </si>
+  <si>
+    <t>OPTIMAX</t>
+  </si>
+  <si>
+    <t>TECHMINDS</t>
+  </si>
+  <si>
+    <t>POWERGEN</t>
+  </si>
+  <si>
+    <t>HUAWEI</t>
   </si>
 </sst>
 </file>
@@ -901,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -930,15 +930,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1256,7 +1254,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1321,240 +1319,240 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="B4" s="11">
         <v>516306</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>17</v>
+        <v>241</v>
       </c>
       <c r="B5" s="11">
         <v>514807</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11">
         <v>516301</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>24</v>
+        <v>242</v>
       </c>
       <c r="B7" s="11">
         <v>522921</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>27</v>
+        <v>243</v>
       </c>
       <c r="B8" s="11">
         <v>516311</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>244</v>
       </c>
       <c r="B9" s="11">
         <v>516300</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="B10" s="11">
         <v>516303</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>37</v>
+        <v>246</v>
       </c>
       <c r="B11" s="11">
         <v>516305</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>41</v>
+        <v>247</v>
       </c>
       <c r="B12" s="11">
         <v>516302</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="B13" s="11">
         <v>516315</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>49</v>
+        <v>249</v>
       </c>
       <c r="B14" s="11">
         <v>516312</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B15" s="11">
         <v>516304</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="B16" s="11">
         <v>520027</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B17" s="11">
         <v>516294</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1568,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864005FC-FDC6-4E63-9CE0-D0AB8CFD1612}">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1580,35 +1578,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -1616,122 +1614,122 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>5.28</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>5.28</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>8.8000000000000007</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>17.600000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>23.23</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>23.23</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1739,10 +1737,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>26.4</v>
@@ -1750,10 +1748,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>26.4</v>
@@ -1761,10 +1759,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C15">
         <v>30.8</v>
@@ -1772,24 +1770,24 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>36.96</v>
@@ -1797,10 +1795,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C18">
         <v>36.96</v>
@@ -1808,38 +1806,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>45</v>
@@ -1847,80 +1845,80 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>54.4</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>54.4</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>59.63</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>59.63</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C27">
         <v>64.010000000000005</v>
@@ -1928,10 +1926,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C28">
         <v>75</v>
@@ -1939,52 +1937,52 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C29">
         <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C30">
         <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C31">
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1992,10 +1990,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -2003,10 +2001,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -2014,24 +2012,24 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>150</v>
@@ -2039,10 +2037,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C37">
         <v>150</v>
@@ -2050,10 +2048,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C38">
         <v>200</v>
@@ -2061,10 +2059,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C39">
         <v>250</v>
@@ -2072,24 +2070,24 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>264</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C41">
         <v>352</v>
@@ -2097,10 +2095,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C42">
         <v>366.08</v>
@@ -2108,10 +2106,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C43">
         <v>385.65</v>
@@ -2119,24 +2117,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>440</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>440</v>
@@ -2144,10 +2142,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>440</v>
@@ -2155,10 +2153,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>440</v>
@@ -2166,10 +2164,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C48">
         <v>488.4</v>
@@ -2177,38 +2175,38 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>528</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>556.82000000000005</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C51">
         <v>600</v>
@@ -2216,24 +2214,24 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>610.72</v>
       </c>
       <c r="D52" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>660</v>
@@ -2241,10 +2239,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C54">
         <v>800</v>
@@ -2252,38 +2250,38 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C55">
         <v>880</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C56">
         <v>880</v>
       </c>
       <c r="D56" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C57">
         <v>880</v>
@@ -2291,24 +2289,24 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C58">
         <v>910</v>
       </c>
       <c r="D58" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C59" s="7">
         <v>1200</v>
@@ -2316,10 +2314,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C60" s="7">
         <v>1200</v>
@@ -2327,10 +2325,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C61" s="7">
         <v>1250</v>
@@ -2338,10 +2336,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C62" s="7">
         <v>1250</v>
@@ -2349,24 +2347,24 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C63" s="7">
         <v>1250</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C64" s="7">
         <v>1320</v>
@@ -2374,24 +2372,24 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C65" s="7">
         <v>1500</v>
       </c>
       <c r="D65" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C66" s="7">
         <v>1500</v>
@@ -2399,10 +2397,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C67" s="7">
         <v>1628</v>
@@ -2410,38 +2408,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C68" s="7">
         <v>1800</v>
       </c>
       <c r="D68" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C69" s="7">
         <v>1800</v>
       </c>
       <c r="D69" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C70" s="7">
         <v>2000</v>
@@ -2449,10 +2447,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C71" s="7">
         <v>2000</v>
@@ -2460,10 +2458,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C72" s="7">
         <v>2000</v>
@@ -2471,10 +2469,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C73" s="7">
         <v>2050</v>
@@ -2482,10 +2480,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C74" s="7">
         <v>2100</v>
@@ -2493,24 +2491,24 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C75" s="7">
         <v>2200</v>
       </c>
       <c r="D75" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C76" s="7">
         <v>2200</v>
@@ -2518,38 +2516,38 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B77" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C77" s="7">
         <v>2200</v>
       </c>
       <c r="D77" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C78" s="7">
         <v>2300</v>
       </c>
       <c r="D78" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C79" s="7">
         <v>2500</v>
@@ -2557,10 +2555,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C80" s="7">
         <v>2500</v>
@@ -2568,10 +2566,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C81" s="7">
         <v>2500</v>
@@ -2579,10 +2577,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C82" s="7">
         <v>2640</v>
@@ -2590,10 +2588,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B83" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C83" s="7">
         <v>2640</v>
@@ -2601,10 +2599,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C84" s="7">
         <v>2640</v>
@@ -2612,10 +2610,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B85" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C85" s="7">
         <v>2640</v>
@@ -2623,24 +2621,24 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C86" s="7">
         <v>2660</v>
       </c>
       <c r="D86" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C87" s="7">
         <v>3000</v>
@@ -2648,10 +2646,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C88" s="7">
         <v>3000</v>
@@ -2659,10 +2657,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C89" s="7">
         <v>3000</v>
@@ -2670,24 +2668,24 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7">
         <v>3300</v>
       </c>
       <c r="D90" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C91" s="7">
         <v>3500</v>
@@ -2695,10 +2693,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C92" s="7">
         <v>3500</v>
@@ -2706,10 +2704,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C93" s="7">
         <v>3520</v>
@@ -2717,24 +2715,24 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C94" s="7">
         <v>3960</v>
       </c>
       <c r="D94" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B95" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C95" s="7">
         <v>4000</v>
@@ -2742,10 +2740,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C96" s="7">
         <v>4000</v>
@@ -2753,10 +2751,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C97" s="7">
         <v>4000</v>
@@ -2764,10 +2762,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C98" s="7">
         <v>4000</v>
@@ -2775,24 +2773,24 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C99" s="7">
         <v>4400</v>
       </c>
       <c r="D99" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C100" s="7">
         <v>4500</v>
@@ -2800,10 +2798,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C101" s="7">
         <v>4500</v>
@@ -2811,10 +2809,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C102" s="7">
         <v>5000</v>
@@ -2822,10 +2820,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C103" s="7">
         <v>5000</v>
@@ -2833,10 +2831,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C104" s="7">
         <v>5000</v>
@@ -2844,24 +2842,24 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B105" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C105" s="7">
         <v>5280</v>
       </c>
       <c r="D105" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B106" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C106" s="7">
         <v>7500</v>
@@ -2869,10 +2867,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C107" s="7">
         <v>7500</v>
@@ -2880,10 +2878,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B108" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C108" s="7">
         <v>8000</v>
@@ -2891,10 +2889,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C109" s="7">
         <v>8000</v>
@@ -2902,10 +2900,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B110" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C110" s="7">
         <v>8500</v>
@@ -2913,10 +2911,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C111" s="7">
         <v>8800</v>
@@ -2924,24 +2922,24 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B112" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C112" s="7">
         <v>9000</v>
       </c>
       <c r="D112" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B113" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C113" s="7">
         <v>9240</v>
@@ -2949,10 +2947,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B114" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C114" s="7">
         <v>9500</v>
@@ -2960,10 +2958,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B115" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C115" s="7">
         <v>10500</v>
@@ -2971,10 +2969,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B116" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C116" s="7">
         <v>10500</v>
@@ -2982,24 +2980,24 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C117" s="7">
         <v>11000</v>
       </c>
       <c r="D117" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B118" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C118" s="7">
         <v>11000</v>
@@ -3007,24 +3005,24 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C119" s="7">
         <v>11000</v>
       </c>
       <c r="D119" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B120" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C120" s="7">
         <v>13200</v>
@@ -3032,10 +3030,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C121" s="7">
         <v>13200</v>
@@ -3043,38 +3041,38 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C122" s="7">
         <v>13500</v>
       </c>
       <c r="D122" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B123" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C123" s="7">
         <v>13500</v>
       </c>
       <c r="D123" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B124" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C124" s="7">
         <v>14000</v>
@@ -3082,10 +3080,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B125" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C125" s="7">
         <v>15500</v>
@@ -3093,10 +3091,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="B126" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C126" s="7">
         <v>15840</v>
@@ -3104,10 +3102,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B127" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C127" s="7">
         <v>19500</v>
@@ -3115,10 +3113,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C128" s="7">
         <v>19580</v>
@@ -3126,10 +3124,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B129" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C129" s="7">
         <v>20000</v>
@@ -3137,10 +3135,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B130" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C130" s="7">
         <v>20000</v>
@@ -3148,10 +3146,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B131" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C131" s="7">
         <v>20000</v>
@@ -3159,10 +3157,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B132" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C132" s="7">
         <v>20000</v>
@@ -3170,10 +3168,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B133" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C133" s="7">
         <v>23760</v>
@@ -3181,10 +3179,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B134" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C134" s="7">
         <v>24500</v>
@@ -3192,24 +3190,24 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B135" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C135" s="7">
         <v>30800</v>
       </c>
       <c r="D135" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B136" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C136" s="7">
         <v>36500</v>
@@ -3217,10 +3215,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B137" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C137" s="7">
         <v>45760</v>
@@ -3228,10 +3226,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B138" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C138" s="7">
         <v>47520</v>
@@ -3239,10 +3237,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B139" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C139" s="7">
         <v>88000</v>
@@ -3250,10 +3248,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B140" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C140" s="7">
         <v>95040</v>
@@ -3261,10 +3259,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B141" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C141" s="7">
         <v>132000</v>
@@ -3278,171 +3276,240 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7D0387-9D33-42A7-95B3-3BA9813FB715}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.81640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="8.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="48.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+    <row r="1" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="12"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="28" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3451,21 +3518,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5B91-39BE-4885-A0A9-44D289EC2A66}">
-  <dimension ref="C2:F2"/>
+  <dimension ref="E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="12" style="16" customWidth="1"/>
-    <col min="6" max="6" width="52" style="14" customWidth="1"/>
-    <col min="7" max="8" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.90625" customWidth="1"/>
+    <col min="2" max="4" width="9.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="35.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" customWidth="1"/>
     <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1796875" customWidth="1"/>
     <col min="11" max="11" width="10.7265625" customWidth="1"/>
@@ -3473,7 +3539,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E2" s="15"/>
+      <c r="E2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Combine all pdf data extraction activities under one Use Browser Activity. Added some delays between actvitis to ensure excel file is available for read/write purposes.
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df2dc9a4c3afcdea/Enterprise Business Services/Projects/Automation/RPA/Capstone-Project-PR-Raising/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{313948B6-BDCC-4361-8F1F-2DCF3F1DC5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C85E1D-73FA-489A-AE79-EE60CC216505}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{313948B6-BDCC-4361-8F1F-2DCF3F1DC5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED24F4C9-C0A6-441C-B37E-3781C46DDE15}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </bookViews>
   <sheets>
     <sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -84,6 +84,9 @@
     <t>Agreement 516313</t>
   </si>
   <si>
+    <t>KINDE</t>
+  </si>
+  <si>
     <t>KINDE ENGINEERING WORKS LIMITED</t>
   </si>
   <si>
@@ -93,6 +96,9 @@
     <t>Agreement 516306</t>
   </si>
   <si>
+    <t>CAMUSAT</t>
+  </si>
+  <si>
     <t>CAMUSAT KENYA LIMITED</t>
   </si>
   <si>
@@ -111,24 +117,36 @@
     <t>Agreement 516301</t>
   </si>
   <si>
+    <t>EXTRA D</t>
+  </si>
+  <si>
     <t>EXTRA DIMENSIONS COMPANY LIMITED</t>
   </si>
   <si>
     <t>Agreement 522921</t>
   </si>
   <si>
+    <t>TETRANET</t>
+  </si>
+  <si>
     <t>TETRANET SERVICES LIMITED</t>
   </si>
   <si>
     <t>Agreement 516311</t>
   </si>
   <si>
+    <t>ADRIAN</t>
+  </si>
+  <si>
     <t>ADRIAN KENYA LIMITED</t>
   </si>
   <si>
     <t>Agreement 516300</t>
   </si>
   <si>
+    <t>PAVICON</t>
+  </si>
+  <si>
     <t>PAVICON (K) LIMITED</t>
   </si>
   <si>
@@ -138,6 +156,9 @@
     <t>Agreement 516303</t>
   </si>
   <si>
+    <t>HATIKVAH</t>
+  </si>
+  <si>
     <t>HATIKVAH COMMUNICATIONS &amp; GENERAL ENGINEERING LIMITED</t>
   </si>
   <si>
@@ -147,6 +168,9 @@
     <t>Agreement 516305</t>
   </si>
   <si>
+    <t>OPTIMAX</t>
+  </si>
+  <si>
     <t>OPTIMAX GROUP LIMITED</t>
   </si>
   <si>
@@ -156,6 +180,9 @@
     <t>Agreement 516302</t>
   </si>
   <si>
+    <t>TECHMINDS</t>
+  </si>
+  <si>
     <t>TECHMINDS TECHNOLOGIES</t>
   </si>
   <si>
@@ -165,6 +192,9 @@
     <t>Agreement 516315</t>
   </si>
   <si>
+    <t>POWERGEN</t>
+  </si>
+  <si>
     <t>POWERGEN TECHNOLOGIES LTD</t>
   </si>
   <si>
@@ -180,6 +210,9 @@
     <t>Agreement 516304</t>
   </si>
   <si>
+    <t>HUAWEI</t>
+  </si>
+  <si>
     <t>HUAWEI TECHNOLOGIES(KENYA) CO. LTD</t>
   </si>
   <si>
@@ -763,39 +796,6 @@
   </si>
   <si>
     <t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</t>
-  </si>
-  <si>
-    <t>KINDE</t>
-  </si>
-  <si>
-    <t>CAMUSAT</t>
-  </si>
-  <si>
-    <t>EXTRA D</t>
-  </si>
-  <si>
-    <t>TETRANET</t>
-  </si>
-  <si>
-    <t>ADRIAN</t>
-  </si>
-  <si>
-    <t>PAVICON</t>
-  </si>
-  <si>
-    <t>HATIKVAH</t>
-  </si>
-  <si>
-    <t>OPTIMAX</t>
-  </si>
-  <si>
-    <t>TECHMINDS</t>
-  </si>
-  <si>
-    <t>POWERGEN</t>
-  </si>
-  <si>
-    <t>HUAWEI</t>
   </si>
 </sst>
 </file>
@@ -1319,240 +1319,240 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>240</v>
+        <v>13</v>
       </c>
       <c r="B4" s="11">
         <v>516306</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="B5" s="11">
         <v>514807</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="11">
         <v>516301</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>242</v>
+        <v>24</v>
       </c>
       <c r="B7" s="11">
         <v>522921</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>243</v>
+        <v>27</v>
       </c>
       <c r="B8" s="11">
         <v>516311</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="B9" s="11">
         <v>516300</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>245</v>
+        <v>33</v>
       </c>
       <c r="B10" s="11">
         <v>516303</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>246</v>
+        <v>37</v>
       </c>
       <c r="B11" s="11">
         <v>516305</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>247</v>
+        <v>41</v>
       </c>
       <c r="B12" s="11">
         <v>516302</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="B13" s="11">
         <v>516315</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>249</v>
+        <v>49</v>
       </c>
       <c r="B14" s="11">
         <v>516312</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B15" s="11">
         <v>516304</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="B16" s="11">
         <v>520027</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B17" s="11">
         <v>516294</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1578,35 +1578,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -1614,122 +1614,122 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>5.28</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>5.28</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>8.8000000000000007</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>17.600000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <v>23.23</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>23.23</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C13">
         <v>26.4</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C14">
         <v>26.4</v>
@@ -1759,10 +1759,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>30.8</v>
@@ -1770,24 +1770,24 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>36.96</v>
@@ -1795,10 +1795,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C18">
         <v>36.96</v>
@@ -1806,38 +1806,38 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C21">
         <v>45</v>
@@ -1845,80 +1845,80 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C22">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>54.4</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C24">
         <v>54.4</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <v>59.63</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C26">
         <v>59.63</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C27">
         <v>64.010000000000005</v>
@@ -1926,10 +1926,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C28">
         <v>75</v>
@@ -1937,52 +1937,52 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C29">
         <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C30">
         <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C31">
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -2012,24 +2012,24 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C35">
         <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C36">
         <v>150</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C37">
         <v>150</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C38">
         <v>200</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C39">
         <v>250</v>
@@ -2070,24 +2070,24 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C40">
         <v>264</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C41">
         <v>352</v>
@@ -2095,10 +2095,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C42">
         <v>366.08</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C43">
         <v>385.65</v>
@@ -2117,24 +2117,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C44">
         <v>440</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C45">
         <v>440</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C46">
         <v>440</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C47">
         <v>440</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C48">
         <v>488.4</v>
@@ -2175,38 +2175,38 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C49">
         <v>528</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C50">
         <v>556.82000000000005</v>
       </c>
       <c r="D50" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C51">
         <v>600</v>
@@ -2214,24 +2214,24 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C52">
         <v>610.72</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C53">
         <v>660</v>
@@ -2239,10 +2239,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C54">
         <v>800</v>
@@ -2250,38 +2250,38 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C55">
         <v>880</v>
       </c>
       <c r="D55" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C56">
         <v>880</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C57">
         <v>880</v>
@@ -2289,24 +2289,24 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C58">
         <v>910</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C59" s="7">
         <v>1200</v>
@@ -2314,10 +2314,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C60" s="7">
         <v>1200</v>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C61" s="7">
         <v>1250</v>
@@ -2336,10 +2336,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C62" s="7">
         <v>1250</v>
@@ -2347,24 +2347,24 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C63" s="7">
         <v>1250</v>
       </c>
       <c r="D63" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C64" s="7">
         <v>1320</v>
@@ -2372,24 +2372,24 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C65" s="7">
         <v>1500</v>
       </c>
       <c r="D65" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C66" s="7">
         <v>1500</v>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C67" s="7">
         <v>1628</v>
@@ -2408,38 +2408,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C68" s="7">
         <v>1800</v>
       </c>
       <c r="D68" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C69" s="7">
         <v>1800</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C70" s="7">
         <v>2000</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C71" s="7">
         <v>2000</v>
@@ -2458,10 +2458,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C72" s="7">
         <v>2000</v>
@@ -2469,10 +2469,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C73" s="7">
         <v>2050</v>
@@ -2480,10 +2480,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C74" s="7">
         <v>2100</v>
@@ -2491,24 +2491,24 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C75" s="7">
         <v>2200</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C76" s="7">
         <v>2200</v>
@@ -2516,38 +2516,38 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C77" s="7">
         <v>2200</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C78" s="7">
         <v>2300</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C79" s="7">
         <v>2500</v>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B80" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C80" s="7">
         <v>2500</v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C81" s="7">
         <v>2500</v>
@@ -2577,10 +2577,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C82" s="7">
         <v>2640</v>
@@ -2588,10 +2588,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B83" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C83" s="7">
         <v>2640</v>
@@ -2599,10 +2599,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C84" s="7">
         <v>2640</v>
@@ -2610,10 +2610,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C85" s="7">
         <v>2640</v>
@@ -2621,24 +2621,24 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B86" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C86" s="7">
         <v>2660</v>
       </c>
       <c r="D86" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B87" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C87" s="7">
         <v>3000</v>
@@ -2646,10 +2646,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C88" s="7">
         <v>3000</v>
@@ -2657,10 +2657,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B89" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C89" s="7">
         <v>3000</v>
@@ -2668,24 +2668,24 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C90" s="7">
         <v>3300</v>
       </c>
       <c r="D90" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C91" s="7">
         <v>3500</v>
@@ -2693,10 +2693,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B92" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C92" s="7">
         <v>3500</v>
@@ -2704,10 +2704,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B93" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C93" s="7">
         <v>3520</v>
@@ -2715,24 +2715,24 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B94" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C94" s="7">
         <v>3960</v>
       </c>
       <c r="D94" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C95" s="7">
         <v>4000</v>
@@ -2740,10 +2740,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C96" s="7">
         <v>4000</v>
@@ -2751,10 +2751,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B97" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C97" s="7">
         <v>4000</v>
@@ -2762,10 +2762,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B98" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C98" s="7">
         <v>4000</v>
@@ -2773,24 +2773,24 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C99" s="7">
         <v>4400</v>
       </c>
       <c r="D99" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B100" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C100" s="7">
         <v>4500</v>
@@ -2798,10 +2798,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B101" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C101" s="7">
         <v>4500</v>
@@ -2809,10 +2809,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C102" s="7">
         <v>5000</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B103" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C103" s="7">
         <v>5000</v>
@@ -2831,10 +2831,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B104" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C104" s="7">
         <v>5000</v>
@@ -2842,24 +2842,24 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B105" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C105" s="7">
         <v>5280</v>
       </c>
       <c r="D105" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="B106" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C106" s="7">
         <v>7500</v>
@@ -2867,10 +2867,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B107" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C107" s="7">
         <v>7500</v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B108" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C108" s="7">
         <v>8000</v>
@@ -2889,10 +2889,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B109" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C109" s="7">
         <v>8000</v>
@@ -2900,10 +2900,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B110" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C110" s="7">
         <v>8500</v>
@@ -2911,10 +2911,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B111" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C111" s="7">
         <v>8800</v>
@@ -2922,24 +2922,24 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C112" s="7">
         <v>9000</v>
       </c>
       <c r="D112" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="B113" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C113" s="7">
         <v>9240</v>
@@ -2947,10 +2947,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B114" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C114" s="7">
         <v>9500</v>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="B115" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C115" s="7">
         <v>10500</v>
@@ -2969,10 +2969,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="B116" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C116" s="7">
         <v>10500</v>
@@ -2980,24 +2980,24 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B117" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C117" s="7">
         <v>11000</v>
       </c>
       <c r="D117" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="B118" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C118" s="7">
         <v>11000</v>
@@ -3005,24 +3005,24 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C119" s="7">
         <v>11000</v>
       </c>
       <c r="D119" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C120" s="7">
         <v>13200</v>
@@ -3030,10 +3030,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C121" s="7">
         <v>13200</v>
@@ -3041,38 +3041,38 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B122" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C122" s="7">
         <v>13500</v>
       </c>
       <c r="D122" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B123" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C123" s="7">
         <v>13500</v>
       </c>
       <c r="D123" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="B124" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C124" s="7">
         <v>14000</v>
@@ -3080,10 +3080,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="B125" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C125" s="7">
         <v>15500</v>
@@ -3091,10 +3091,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="B126" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C126" s="7">
         <v>15840</v>
@@ -3102,10 +3102,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B127" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C127" s="7">
         <v>19500</v>
@@ -3113,10 +3113,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="B128" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C128" s="7">
         <v>19580</v>
@@ -3124,10 +3124,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B129" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C129" s="7">
         <v>20000</v>
@@ -3135,10 +3135,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="B130" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C130" s="7">
         <v>20000</v>
@@ -3146,10 +3146,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B131" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C131" s="7">
         <v>20000</v>
@@ -3157,10 +3157,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="B132" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C132" s="7">
         <v>20000</v>
@@ -3168,10 +3168,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B133" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C133" s="7">
         <v>23760</v>
@@ -3179,10 +3179,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="B134" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C134" s="7">
         <v>24500</v>
@@ -3190,24 +3190,24 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="B135" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C135" s="7">
         <v>30800</v>
       </c>
       <c r="D135" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B136" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C136" s="7">
         <v>36500</v>
@@ -3215,10 +3215,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="B137" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C137" s="7">
         <v>45760</v>
@@ -3226,10 +3226,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="B138" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C138" s="7">
         <v>47520</v>
@@ -3237,10 +3237,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="B139" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C139" s="7">
         <v>88000</v>
@@ -3248,10 +3248,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B140" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C140" s="7">
         <v>95040</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="B141" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C141" s="7">
         <v>132000</v>
@@ -3278,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7D0387-9D33-42A7-95B3-3BA9813FB715}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3445,10 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="12"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="12"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -3520,8 +3523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BA5B91-39BE-4885-A0A9-44D289EC2A66}">
   <dimension ref="E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>